<commit_message>
feat: capture invoice and return
</commit_message>
<xml_diff>
--- a/dados_fatura.xlsx
+++ b/dados_fatura.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E148"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2022-12-02</t>
+          <t>2022-12-09</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -474,7 +474,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>11:10:01</t>
+          <t>11:18:45</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CONSORCIO MUNHOZ 1 ENERGIARURAL B BOM JARDIM, 0 - Sítio Paineiras, Estrada 37620000B BOM JARDIMMUNHOZ (AG: 316)</t>
+          <t>PEDRO MONTELEONE VEICULOS E MOTORES LIMITADAAVENIDA ORLANDO ZANCANER, 1911 -   15801120 - 15801120INDEFINIDOCATANDUVA (AG: 401)</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MTV-MOD.TARIFÁRIA VERDE / A3AINDUSTRIAL / INDUSTRIAL</t>
+          <t>MTC-CONVENCIONAL BAIXA TENSÃO / B3COMERCIAL / COMERCIAL</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>082 - 3016 - 010 - 0050W9007777164</t>
+          <t>003 - 4001 - 070 - 1790W9004861512</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0002598964-2022-09-4</t>
+          <t>4025957-2022-10-5</t>
         </is>
       </c>
     </row>
@@ -589,11 +589,11 @@
         <v>211</v>
       </c>
       <c r="D9" t="n">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LIGAÇÃO:DOM.  BANC.:CNPJ/CPF: 41.628.717/0001-60</t>
+          <t>LIGAÇÃO:DOM.  BANC.:CNPJ/CPF/RANI: 47.069.869/0001-56Insc. Est.: 260000880111</t>
         </is>
       </c>
     </row>
@@ -603,14 +603,14 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>363</v>
+        <v>398</v>
       </c>
       <c r="D10" t="n">
-        <v>750</v>
+        <v>765</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.Rua Capitão Soares, 667, CENTROCAMBUI - MG CEP 37600-000CNPJ 07.282.377/0081-04     Insc. Est. 002522747.04-56Nota Fiscal/Conta de Energia ElétricaSérie: B1   NF: 000.016.131Reimpressão da NF/CEE, nos termos do Regime Especial/PTA nº45.000015601-58 - SEF/MG</t>
+          <t>ENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.Rod Assis Chateaubriand S/N, KM 455 - Bairro: Vila MariaPRESIDENTE PRUDENTE – SP CEP 19053-680CNPJ 07.282.377/0001-20     Insc. Est. 562.408.684.115Nota Fiscal/Conta de Energia ElétricaSérie: U   NF: 040.936.936</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Emissão: 03/10/2022</t>
+          <t>Emissão: 10/10/2022</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0002598964-1</t>
+          <t>0004025957-4</t>
         </is>
       </c>
     </row>
@@ -671,14 +671,14 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D14" t="n">
         <v>674</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Setembro/2022</t>
+          <t>Outubro/2022</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>06/10/2022</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -705,14 +705,14 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D16" t="n">
         <v>674</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>31/10/2022</t>
+          <t>07/11/2022</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>9/2598964-1</t>
+          <t>9/4025957-4</t>
         </is>
       </c>
     </row>
@@ -742,11 +742,11 @@
         <v>34</v>
       </c>
       <c r="D18" t="n">
-        <v>568</v>
+        <v>608</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CCI Descrição0601 Consumo em kWh - Ponta0601 Energia Atv Injetada - Ponta0601 Consumo em kWh - Fora Ponta06010601 Energia Reativa Exced em KWh - Ponta0601 Energia Reativa Exced em KWh - FPonta0602 Demanda de Potência Medida - Fora Ponta0602 Demanda Potência Não Consumida - F Ponta</t>
+          <t>CCI Descrição0601 Consumo em kWh0601 Energia Atv Injetada0601 Dif. Custo Disp. Res. 482.</t>
         </is>
       </c>
     </row>
@@ -756,14 +756,14 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="D19" t="n">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Energia Atv Injetada - Fora Ponta</t>
+          <t>Quantidade3.792,003.792,00100,00</t>
         </is>
       </c>
     </row>
@@ -773,14 +773,14 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>50</v>
+        <v>217</v>
       </c>
       <c r="D20" t="n">
-        <v>560</v>
+        <v>608</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LANÇAMENTOS E SERVIÇOS</t>
+          <t>Tarifa s/Tributos0,6219500,6219500,621950</t>
         </is>
       </c>
     </row>
@@ -790,14 +790,14 @@
         <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>34</v>
+        <v>257</v>
       </c>
       <c r="D21" t="n">
-        <v>552</v>
+        <v>608</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0807 Contrib de Ilum Pub</t>
+          <t>Tarifa c/Tributos0,7879400,7073500,787940</t>
         </is>
       </c>
     </row>
@@ -807,14 +807,14 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>176</v>
+        <v>293</v>
       </c>
       <c r="D22" t="n">
-        <v>568</v>
+        <v>608</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Quantidade181,65181,651.159,201.159,2023,10197,408,40824,10</t>
+          <t>Valor Total(R$)2.987,88-2.682,2978,79</t>
         </is>
       </c>
     </row>
@@ -824,14 +824,14 @@
         <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>254</v>
+        <v>332</v>
       </c>
       <c r="D23" t="n">
-        <v>568</v>
+        <v>608</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tarifa c/Tributos1,6162401,6162400,4498400,4498400,3402200,34022020,18491020,184910</t>
+          <t>Base Calc.ICMS(R$)2.987,88-1.290,1378,79</t>
         </is>
       </c>
     </row>
@@ -841,14 +841,14 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>293</v>
+        <v>366</v>
       </c>
       <c r="D24" t="n">
-        <v>568</v>
+        <v>608</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Valor Total(R$)293,59-293,59521,47-521,477,8567,16169,5516.634,38</t>
+          <t>%Aliq.ICMS181818</t>
         </is>
       </c>
     </row>
@@ -858,14 +858,14 @@
         <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>332</v>
+        <v>396</v>
       </c>
       <c r="D25" t="n">
-        <v>568</v>
+        <v>608</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Base Calc.ICMS(R$)95,42-95,42374,86-374,867,8567,160,000,00</t>
+          <t>ICMS (R$)537,81-232,2214,18</t>
         </is>
       </c>
     </row>
@@ -875,14 +875,14 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>366</v>
+        <v>428</v>
       </c>
       <c r="D26" t="n">
-        <v>568</v>
+        <v>641</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>%Aliq.ICMS181818181818180</t>
+          <t>Base Calc.</t>
         </is>
       </c>
     </row>
@@ -892,14 +892,14 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>308</v>
+        <v>420</v>
       </c>
       <c r="D27" t="n">
-        <v>552</v>
+        <v>608</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>46,17</t>
+          <t>PIS/COFINS (R$)2.450,06-2.450,0664,61</t>
         </is>
       </c>
     </row>
@@ -909,14 +909,14 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>350</v>
+        <v>474</v>
       </c>
       <c r="D28" t="n">
-        <v>552</v>
+        <v>608</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>PIS (R$) COFINS(R$)(3,0729%)75,29-75,291,98</t>
         </is>
       </c>
     </row>
@@ -926,14 +926,14 @@
         <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>376</v>
+        <v>470</v>
       </c>
       <c r="D29" t="n">
-        <v>552</v>
+        <v>608</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>(0,6671%)16,34-16,340,43</t>
         </is>
       </c>
     </row>
@@ -943,14 +943,14 @@
         <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>400</v>
+        <v>35</v>
       </c>
       <c r="D30" t="n">
-        <v>568</v>
+        <v>431</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>ICMS (R$)17,18-17,1867,47-67,471,4112,090,000,00</t>
+          <t>CCI: Código de Classificação do Item</t>
         </is>
       </c>
     </row>
@@ -960,14 +960,14 @@
         <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>405</v>
+        <v>248</v>
       </c>
       <c r="D31" t="n">
-        <v>552</v>
+        <v>431</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>Total:</t>
         </is>
       </c>
     </row>
@@ -977,14 +977,14 @@
         <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>428</v>
+        <v>304</v>
       </c>
       <c r="D32" t="n">
-        <v>641</v>
+        <v>431</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Base Calc.</t>
+          <t>384,38</t>
         </is>
       </c>
     </row>
@@ -994,14 +994,14 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>420</v>
+        <v>338</v>
       </c>
       <c r="D33" t="n">
-        <v>568</v>
+        <v>431</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>PIS/COFINS (R$)276,41-276,41453,99-453,996,4455,07169,5516.634,38</t>
+          <t>1.776,54</t>
         </is>
       </c>
     </row>
@@ -1011,14 +1011,14 @@
         <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>474</v>
+        <v>398</v>
       </c>
       <c r="D34" t="n">
-        <v>568</v>
+        <v>431</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>PIS (R$) COFINS(R$)(3,0729%)8,49-8,4913,95-13,950,201,695,21511,16</t>
+          <t>319,77</t>
         </is>
       </c>
     </row>
@@ -1028,14 +1028,14 @@
         <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="D35" t="n">
-        <v>568</v>
+        <v>431</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>(0,6671%)1,84-1,843,03-3,030,040,371,13110,97</t>
+          <t>64,61</t>
         </is>
       </c>
     </row>
@@ -1045,14 +1045,14 @@
         <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>453</v>
+        <v>485</v>
       </c>
       <c r="D36" t="n">
-        <v>552</v>
+        <v>431</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>0,43</t>
         </is>
       </c>
     </row>
@@ -1062,14 +1062,14 @@
         <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>485</v>
+        <v>525</v>
       </c>
       <c r="D37" t="n">
-        <v>552</v>
+        <v>431</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,98</t>
         </is>
       </c>
     </row>
@@ -1079,14 +1079,14 @@
         <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>525</v>
+        <v>63</v>
       </c>
       <c r="D38" t="n">
-        <v>552</v>
+        <v>395</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>DISCRIMINAÇÃO</t>
         </is>
       </c>
     </row>
@@ -1096,14 +1096,14 @@
         <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D39" t="n">
-        <v>431</v>
+        <v>355</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>CCI: Código de Classificação do Item</t>
+          <t>SERVIÇO DISTRIBUIÇÃOCOMPRA DE ENERGIASERVIÇO DE TRANSMISSÃOENCARGOS SETORIAISIMPOSTOS DIRETOS E ENCARGOSOUTROS SERVIÇOS</t>
         </is>
       </c>
     </row>
@@ -1113,14 +1113,14 @@
         <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>248</v>
+        <v>75</v>
       </c>
       <c r="D40" t="n">
-        <v>431</v>
+        <v>348</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Total:</t>
+          <t>TOTAL</t>
         </is>
       </c>
     </row>
@@ -1130,14 +1130,14 @@
         <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>296</v>
+        <v>210</v>
       </c>
       <c r="D41" t="n">
-        <v>431</v>
+        <v>388</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>16.925,11</t>
+          <t>21/10/2022</t>
         </is>
       </c>
     </row>
@@ -1147,14 +1147,14 @@
         <v>4</v>
       </c>
       <c r="C42" t="n">
-        <v>346</v>
+        <v>382</v>
       </c>
       <c r="D42" t="n">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>75,01</t>
+          <t>R$ 384,38</t>
         </is>
       </c>
     </row>
@@ -1164,14 +1164,14 @@
         <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>402</v>
+        <v>137</v>
       </c>
       <c r="D43" t="n">
-        <v>431</v>
+        <v>348</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>13,50</t>
+          <t>VALOR (R$)12,7028,575,8815,05322,180,00384,38</t>
         </is>
       </c>
     </row>
@@ -1181,14 +1181,14 @@
         <v>4</v>
       </c>
       <c r="C44" t="n">
-        <v>440</v>
+        <v>172</v>
       </c>
       <c r="D44" t="n">
-        <v>431</v>
+        <v>348</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>16.865,44</t>
+          <t>%3,307,431,533,9283,820,00100,00</t>
         </is>
       </c>
     </row>
@@ -1198,14 +1198,14 @@
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>478</v>
+        <v>268</v>
       </c>
       <c r="D45" t="n">
-        <v>431</v>
+        <v>327</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>112,51</t>
+          <t>844d.4da2.80bd.c2de.f0fb.fa28.b32a.99a3</t>
         </is>
       </c>
     </row>
@@ -1215,14 +1215,14 @@
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>518</v>
+        <v>210</v>
       </c>
       <c r="D46" t="n">
-        <v>431</v>
+        <v>263</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>518,26</t>
+          <t>00190.00009 03268.923004 42255.211171 4 91450000038438</t>
         </is>
       </c>
     </row>
@@ -1232,14 +1232,14 @@
         <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>63</v>
+        <v>198</v>
       </c>
       <c r="D47" t="n">
-        <v>395</v>
+        <v>263</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>DISCRIMINAÇÃO</t>
+          <t>-9</t>
         </is>
       </c>
     </row>
@@ -1249,14 +1249,14 @@
         <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>37</v>
+        <v>185</v>
       </c>
       <c r="D48" t="n">
-        <v>355</v>
+        <v>263</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>SERVIÇO DISTRIBUIÇÃOCOMPRA DE ENERGIASERVIÇO DE TRANSMISSÃOENCARGOS SETORIAISIMPOSTOS DIRETOS E ENCARGOSOUTROS SERVIÇOS</t>
+          <t>001</t>
         </is>
       </c>
     </row>
@@ -1266,14 +1266,14 @@
         <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D49" t="n">
-        <v>333</v>
+        <v>196</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>VALOR (R$)3.315,117.458,211.534,183.927,17690,440,0016.925,11- Valor Encargo Uso Sist. Distr. (Ref 07/2022): R$15.598,55</t>
+          <t>BANCO DO BRASIL S/ALOCAL DE PAGAMENTOPAGAR PREFERENCIALMENTE NO  BANCO DO BRASIL S/ABENEFICIÁRIOENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.ENDEREÇOROD ASSIS CHATEAUBRIAND S/N, S/N - KM 455 - VILA MARIA - PRESIDENTE PRUDENTE / SP - CEP 19053-680DATA DO DOCUMENTO</t>
         </is>
       </c>
     </row>
@@ -1283,14 +1283,14 @@
         <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="D50" t="n">
-        <v>348</v>
+        <v>196</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>TOTAL</t>
+          <t>ESPÉCIE DOC</t>
         </is>
       </c>
     </row>
@@ -1300,14 +1300,14 @@
         <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>210</v>
+        <v>310</v>
       </c>
       <c r="D51" t="n">
-        <v>388</v>
+        <v>223</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>14/10/2022</t>
+          <t>CNPJ07.282.377/0001-20</t>
         </is>
       </c>
     </row>
@@ -1317,14 +1317,14 @@
         <v>4</v>
       </c>
       <c r="C52" t="n">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D52" t="n">
-        <v>389</v>
+        <v>234</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>R$ 16.925,11</t>
+          <t>VENCIMENTO21/10/2022AG./CÓD.BENEFICIÁRIO</t>
         </is>
       </c>
     </row>
@@ -1334,14 +1334,14 @@
         <v>4</v>
       </c>
       <c r="C53" t="n">
-        <v>172</v>
+        <v>453</v>
       </c>
       <c r="D53" t="n">
-        <v>348</v>
+        <v>267</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>%19,5944,079,0623,204,080,00100,00</t>
+          <t>Promoção 1 Ano Por Nossa Conta</t>
         </is>
       </c>
     </row>
@@ -1351,14 +1351,14 @@
         <v>4</v>
       </c>
       <c r="C54" t="n">
-        <v>269</v>
+        <v>457</v>
       </c>
       <c r="D54" t="n">
-        <v>327</v>
+        <v>260</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>8b43.8610.de33.d965.0afb.f810.cafc.ee5c</t>
+          <t>Pague com QR Code do PIX e</t>
         </is>
       </c>
     </row>
@@ -1368,14 +1368,14 @@
         <v>4</v>
       </c>
       <c r="C55" t="n">
-        <v>210</v>
+        <v>451</v>
       </c>
       <c r="D55" t="n">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>00190.00009 03268.923004 42033.164171 6 91380001692511</t>
+          <t>concorra a 1 Ano de Energia Grátis.Use seu app de pagamento favorito,</t>
         </is>
       </c>
     </row>
@@ -1385,14 +1385,14 @@
         <v>4</v>
       </c>
       <c r="C56" t="n">
-        <v>198</v>
+        <v>453</v>
       </c>
       <c r="D56" t="n">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>-9</t>
+          <t>escolha "Pagar com PIX", leiao QR Code abaixo e cadastre-se:</t>
         </is>
       </c>
     </row>
@@ -1402,14 +1402,14 @@
         <v>4</v>
       </c>
       <c r="C57" t="n">
-        <v>185</v>
+        <v>466</v>
       </c>
       <c r="D57" t="n">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>www.anodeconta.com.br</t>
         </is>
       </c>
     </row>
@@ -1419,14 +1419,14 @@
         <v>4</v>
       </c>
       <c r="C58" t="n">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D58" t="n">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>BANCO DO BRASIL S/ALOCAL DE PAGAMENTOPAGAR PREFERENCIALMENTE NO  BANCO DO BRASIL S/ABENEFICIÁRIOENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.ENDEREÇOROD ASSIS CHATEAUBRIAND S/N, S/N - KM 455 - VILA MARIA - PRESIDENTE PRUDENTE / SP - CEP 19053-680DATA DO DOCUMENTO</t>
+          <t>10/10/2022</t>
         </is>
       </c>
     </row>
@@ -1436,14 +1436,14 @@
         <v>4</v>
       </c>
       <c r="C59" t="n">
-        <v>199</v>
+        <v>38</v>
       </c>
       <c r="D59" t="n">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>ESPÉCIE DOC</t>
+          <t>USO DO BANCO</t>
         </is>
       </c>
     </row>
@@ -1453,14 +1453,14 @@
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>310</v>
+        <v>38</v>
       </c>
       <c r="D60" t="n">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>CNPJ07.282.377/0001-20</t>
+          <t>INSTRUÇÕES</t>
         </is>
       </c>
     </row>
@@ -1470,14 +1470,14 @@
         <v>4</v>
       </c>
       <c r="C61" t="n">
-        <v>373</v>
+        <v>103</v>
       </c>
       <c r="D61" t="n">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>VENCIMENTO14/10/2022AG./CÓD.BENEFICIÁRIO</t>
+          <t>Nº DOCUMENTO4025957-2022-10-5CARTEIRA17</t>
         </is>
       </c>
     </row>
@@ -1487,14 +1487,14 @@
         <v>4</v>
       </c>
       <c r="C62" t="n">
-        <v>393</v>
+        <v>249</v>
       </c>
       <c r="D62" t="n">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3064-3/005292-2</t>
+          <t>ACEITEN</t>
         </is>
       </c>
     </row>
@@ -1504,14 +1504,14 @@
         <v>4</v>
       </c>
       <c r="C63" t="n">
-        <v>453</v>
+        <v>286</v>
       </c>
       <c r="D63" t="n">
-        <v>267</v>
+        <v>187</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Promoção 1 Ano Por Nossa Conta</t>
+          <t>DATA DO PROCESSAMENTO10/10/2022</t>
         </is>
       </c>
     </row>
@@ -1521,14 +1521,14 @@
         <v>4</v>
       </c>
       <c r="C64" t="n">
-        <v>457</v>
+        <v>249</v>
       </c>
       <c r="D64" t="n">
-        <v>260</v>
+        <v>177</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Pague com QR Code do PIX e</t>
+          <t>QUANTIDADE</t>
         </is>
       </c>
     </row>
@@ -1538,14 +1538,14 @@
         <v>4</v>
       </c>
       <c r="C65" t="n">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="D65" t="n">
-        <v>247</v>
+        <v>177</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>concorra a 1 Ano de Energia Grátis.Use seu app de pagamento favorito,</t>
+          <t>VALOR</t>
         </is>
       </c>
     </row>
@@ -1555,14 +1555,14 @@
         <v>4</v>
       </c>
       <c r="C66" t="n">
-        <v>453</v>
+        <v>215</v>
       </c>
       <c r="D66" t="n">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>escolha "Pagar com PIX", leiao QR Code abaixo e cadastre-se:</t>
+          <t>DSESPÉCIER$</t>
         </is>
       </c>
     </row>
@@ -1572,14 +1572,14 @@
         <v>4</v>
       </c>
       <c r="C67" t="n">
-        <v>466</v>
+        <v>38</v>
       </c>
       <c r="D67" t="n">
-        <v>226</v>
+        <v>114</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>www.anodeconta.com.br</t>
+          <t>OS VALORES DA MULTA/JUROS DE MORA POR ATRASO SÓ SERÃO COBRADOSNA PRIMEIRA FATURA APÓS O PAGAMENTO DESTA.TITULO SUJEITO A PROTESTO APÓS O VENCIMENTONÃO ACEITAMOS DEPÓSITO EM CONTA CORRENTE. CASO OCORRA, O MESMO NÃO QUITARÁ ESTA FATURA.</t>
         </is>
       </c>
     </row>
@@ -1589,14 +1589,14 @@
         <v>4</v>
       </c>
       <c r="C68" t="n">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D68" t="n">
-        <v>187</v>
+        <v>68</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>03/10/2022</t>
+          <t>PAGADORPEDRO MONTELEONE VEICULOS E MOTORES LIMITADAAVENIDA ORLANDO ZANCANER, 1911 -   15801120     CATANDUVA (AG: 401)SACADOR/ AVALISTA</t>
         </is>
       </c>
     </row>
@@ -1606,14 +1606,14 @@
         <v>4</v>
       </c>
       <c r="C69" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D69" t="n">
-        <v>177</v>
+        <v>32</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>USO DO BANCO</t>
+          <t>(B{SgDgQtRuB{B{[eLcQ{B{B{LiGsSmOcB{DdMsTbWdQh)</t>
         </is>
       </c>
     </row>
@@ -1623,14 +1623,14 @@
         <v>4</v>
       </c>
       <c r="C70" t="n">
-        <v>38</v>
+        <v>373</v>
       </c>
       <c r="D70" t="n">
-        <v>159</v>
+        <v>214</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>INSTRUÇÕES</t>
+          <t>NOSSO NÚMERO</t>
         </is>
       </c>
     </row>
@@ -1640,14 +1640,14 @@
         <v>4</v>
       </c>
       <c r="C71" t="n">
-        <v>103</v>
+        <v>364</v>
       </c>
       <c r="D71" t="n">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Nº DOCUMENTO2598964-2022-09-4CARTEIRA17</t>
+          <t>32689230042255211</t>
         </is>
       </c>
     </row>
@@ -1657,14 +1657,14 @@
         <v>4</v>
       </c>
       <c r="C72" t="n">
-        <v>249</v>
+        <v>373</v>
       </c>
       <c r="D72" t="n">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ACEITEN</t>
+          <t>(=)VALOR DO DOCUMENTO</t>
         </is>
       </c>
     </row>
@@ -1674,14 +1674,14 @@
         <v>4</v>
       </c>
       <c r="C73" t="n">
-        <v>286</v>
+        <v>373</v>
       </c>
       <c r="D73" t="n">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>DATA DO PROCESSAMENTO03/10/2022</t>
+          <t>384,38(-) DESCONTOS/ ABATIMENTOS</t>
         </is>
       </c>
     </row>
@@ -1691,14 +1691,14 @@
         <v>4</v>
       </c>
       <c r="C74" t="n">
-        <v>249</v>
+        <v>373</v>
       </c>
       <c r="D74" t="n">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>QUANTIDADE</t>
+          <t>(-) OUTRAS DEDUÇÕES</t>
         </is>
       </c>
     </row>
@@ -1708,14 +1708,14 @@
         <v>4</v>
       </c>
       <c r="C75" t="n">
-        <v>333</v>
+        <v>373</v>
       </c>
       <c r="D75" t="n">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>VALOR</t>
+          <t>(+) MORA/ MULTA</t>
         </is>
       </c>
     </row>
@@ -1725,14 +1725,14 @@
         <v>4</v>
       </c>
       <c r="C76" t="n">
-        <v>215</v>
+        <v>373</v>
       </c>
       <c r="D76" t="n">
-        <v>168</v>
+        <v>126</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>DSESPÉCIER$</t>
+          <t>(+) OUTROS ACRÉSCIMOS</t>
         </is>
       </c>
     </row>
@@ -1742,14 +1742,14 @@
         <v>4</v>
       </c>
       <c r="C77" t="n">
-        <v>38</v>
+        <v>373</v>
       </c>
       <c r="D77" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>OS VALORES DA MULTA/JUROS DE MORA POR ATRASO SÓ SERÃO COBRADOSNA PRIMEIRA FATURA APÓS O PAGAMENTO DESTA.TITULO SUJEITO A PROTESTO APÓS O VENCIMENTONÃO ACEITAMOS DEPÓSITO EM CONTA CORRENTE. CASO OCORRA, O MESMO NÃO QUITARÁ ESTA FATURA.</t>
+          <t>(=) VALOR COBRADO</t>
         </is>
       </c>
     </row>
@@ -1759,14 +1759,14 @@
         <v>4</v>
       </c>
       <c r="C78" t="n">
-        <v>38</v>
+        <v>373</v>
       </c>
       <c r="D78" t="n">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>PAGADORCONSORCIO MUNHOZ 1 ENERGIARURAL B BOM JARDIM, 0 - Sítio Paineiras, Estrada 37620000     MUNHOZ (AG: 316)SACADOR/ AVALISTA</t>
+          <t>CPF/CNPJ47.069.869/0001-56</t>
         </is>
       </c>
     </row>
@@ -1776,14 +1776,14 @@
         <v>4</v>
       </c>
       <c r="C79" t="n">
-        <v>39</v>
+        <v>412</v>
       </c>
       <c r="D79" t="n">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>(B{SgHeYcQ{B{SsGjXbQvB{B{LiGsSmOcB{DdLi[bFrQh)</t>
+          <t>CÓD. DE BAIXA</t>
         </is>
       </c>
     </row>
@@ -1793,14 +1793,14 @@
         <v>4</v>
       </c>
       <c r="C80" t="n">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="D80" t="n">
-        <v>214</v>
+        <v>60</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>NOSSO NÚMERO</t>
+          <t>AUTENTICAÇÃO MECÂNICA</t>
         </is>
       </c>
     </row>
@@ -1810,14 +1810,14 @@
         <v>4</v>
       </c>
       <c r="C81" t="n">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="D81" t="n">
-        <v>204</v>
+        <v>32</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>32689230042033164</t>
+          <t>Ficha de Compensação</t>
         </is>
       </c>
     </row>
@@ -1827,14 +1827,14 @@
         <v>4</v>
       </c>
       <c r="C82" t="n">
-        <v>373</v>
+        <v>456</v>
       </c>
       <c r="D82" t="n">
-        <v>195</v>
+        <v>96</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>(=)VALOR DO DOCUMENTO</t>
+          <t>Quer facilidade?Abra sua Conta Voltz - Energisae tenha vantagens exclusivas!</t>
         </is>
       </c>
     </row>
@@ -1844,184 +1844,184 @@
         <v>4</v>
       </c>
       <c r="C83" t="n">
-        <v>373</v>
+        <v>456</v>
       </c>
       <c r="D83" t="n">
-        <v>176</v>
+        <v>76</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>16.925,11(-) DESCONTOS/ ABATIMENTOS</t>
+          <t>Entenda melhor emcontavoltz.com/pix</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr"/>
       <c r="B84" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C84" t="n">
-        <v>373</v>
+        <v>38</v>
       </c>
       <c r="D84" t="n">
-        <v>159</v>
+        <v>784</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>(-) OUTRAS DEDUÇÕES</t>
+          <t>-Censo 2022 - Receba os recenseadores - Responda para o Brasilsaber o que precisa. censo2022.ibge.gov.br.</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr"/>
       <c r="B85" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C85" t="n">
-        <v>373</v>
+        <v>232</v>
       </c>
       <c r="D85" t="n">
-        <v>143</v>
+        <v>790</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>(+) MORA/ MULTA</t>
+          <t>VENCIMENTO</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr"/>
       <c r="B86" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C86" t="n">
-        <v>373</v>
+        <v>277</v>
       </c>
       <c r="D86" t="n">
-        <v>126</v>
+        <v>790</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>(+) OUTROS ACRÉSCIMOS</t>
+          <t>VALOR (R$)</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr"/>
       <c r="B87" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C87" t="n">
-        <v>373</v>
+        <v>324</v>
       </c>
       <c r="D87" t="n">
-        <v>109</v>
+        <v>772</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>(=) VALOR COBRADO</t>
+          <t>Isenção Taxa IP- UC com Mini Geração conforme REH 482/2012.- Saldo Acumulado: 21099. A expirar no próximo ciclo: 0- Leitura confirmada</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr"/>
       <c r="B88" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C88" t="n">
-        <v>373</v>
+        <v>52</v>
       </c>
       <c r="D88" t="n">
-        <v>84</v>
+        <v>536</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>CPF/CNPJ41.628.717/0001-60</t>
+          <t>MÊS/ANOOUT/22SET/22AGO/22JUL/22JUN/22MAI/22ABR/22MAR/22FEV/22JAN/22DEZ/21NOV/21OUT/21</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr"/>
       <c r="B89" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C89" t="n">
-        <v>412</v>
+        <v>99</v>
       </c>
       <c r="D89" t="n">
-        <v>69</v>
+        <v>635</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>CÓD. DE BAIXA</t>
+          <t>CONVENCIONAL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr"/>
       <c r="B90" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C90" t="n">
-        <v>382</v>
+        <v>176</v>
       </c>
       <c r="D90" t="n">
-        <v>60</v>
+        <v>636</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>AUTENTICAÇÃO MECÂNICA</t>
+          <t>PONTA</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr"/>
       <c r="B91" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C91" t="n">
-        <v>373</v>
+        <v>235</v>
       </c>
       <c r="D91" t="n">
-        <v>32</v>
+        <v>635</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Ficha de Compensação</t>
+          <t>INTERMEDIÁRIO</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr"/>
       <c r="B92" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C92" t="n">
-        <v>456</v>
+        <v>301</v>
       </c>
       <c r="D92" t="n">
-        <v>96</v>
+        <v>635</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Quer facilidade?Abra sua Conta Voltz - Energisae tenha vantagens exclusivas!</t>
+          <t>FORA  DE  PONTA</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr"/>
       <c r="B93" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C93" t="n">
-        <v>456</v>
+        <v>184</v>
       </c>
       <c r="D93" t="n">
-        <v>76</v>
+        <v>644</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Entenda melhor emcontavoltz.com/pix</t>
+          <t>HISTÓRICO DE CONSUMO (kWh)</t>
         </is>
       </c>
     </row>
@@ -2031,14 +2031,14 @@
         <v>28</v>
       </c>
       <c r="C94" t="n">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D94" t="n">
-        <v>784</v>
+        <v>536</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>-Censo 2022 - Receba os recenseadores - Responda para o Brasilsaber o que precisa. censo2022.ibge.gov.br.</t>
+          <t>379234333741338234856303876399423613886610198881510455</t>
         </is>
       </c>
     </row>
@@ -2048,14 +2048,14 @@
         <v>28</v>
       </c>
       <c r="C95" t="n">
-        <v>232</v>
+        <v>35</v>
       </c>
       <c r="D95" t="n">
-        <v>790</v>
+        <v>490</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>VENCIMENTO</t>
+          <t>Leitura Anterior:06/09/2022</t>
         </is>
       </c>
     </row>
@@ -2065,14 +2065,14 @@
         <v>28</v>
       </c>
       <c r="C96" t="n">
-        <v>277</v>
+        <v>113</v>
       </c>
       <c r="D96" t="n">
-        <v>790</v>
+        <v>490</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>VALOR (R$)</t>
+          <t>Leitura Atual:07/10/2022</t>
         </is>
       </c>
     </row>
@@ -2082,14 +2082,14 @@
         <v>28</v>
       </c>
       <c r="C97" t="n">
-        <v>324</v>
+        <v>183</v>
       </c>
       <c r="D97" t="n">
-        <v>784</v>
+        <v>490</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>UC com Mini Geração conforme REH 482/2012Saldo Ac: 5(P) 4(FP) A expirar em 10/2022: 0(P) 0(FP)</t>
+          <t>Dias: 31</t>
         </is>
       </c>
     </row>
@@ -2099,14 +2099,14 @@
         <v>28</v>
       </c>
       <c r="C98" t="n">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="D98" t="n">
-        <v>630</v>
+        <v>451</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>PONTA</t>
+          <t>UN.KWHINJ</t>
         </is>
       </c>
     </row>
@@ -2116,14 +2116,14 @@
         <v>28</v>
       </c>
       <c r="C99" t="n">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="D99" t="n">
-        <v>630</v>
+        <v>468</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>FORA  DE  PONTA</t>
+          <t>Posto</t>
         </is>
       </c>
     </row>
@@ -2133,14 +2133,14 @@
         <v>28</v>
       </c>
       <c r="C100" t="n">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="D100" t="n">
-        <v>630</v>
+        <v>451</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>PONTA</t>
+          <t>PP</t>
         </is>
       </c>
     </row>
@@ -2150,14 +2150,14 @@
         <v>28</v>
       </c>
       <c r="C101" t="n">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D101" t="n">
-        <v>630</v>
+        <v>452</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>FORA  DE  PONTA</t>
+          <t>Atual927,00537,00</t>
         </is>
       </c>
     </row>
@@ -2167,14 +2167,14 @@
         <v>28</v>
       </c>
       <c r="C102" t="n">
-        <v>350</v>
+        <v>141</v>
       </c>
       <c r="D102" t="n">
-        <v>630</v>
+        <v>477</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>RESERVADO</t>
+          <t>Dados da leitura</t>
         </is>
       </c>
     </row>
@@ -2184,14 +2184,14 @@
         <v>28</v>
       </c>
       <c r="C103" t="n">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="D103" t="n">
-        <v>551</v>
+        <v>452</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>CONSUMOFATURADO181,65128,10134,401,0512,6013,653,1598,70465,15</t>
+          <t>Anterior853,00431,00</t>
         </is>
       </c>
     </row>
@@ -2201,14 +2201,14 @@
         <v>28</v>
       </c>
       <c r="C104" t="n">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="D104" t="n">
-        <v>520</v>
+        <v>452</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>MÊS/ANOSET/22AGO/22JUL/22JUN/22MAI/22ABR/22MAR/22FEV/22JAN/22DEZ/21NOV/21OUT/21SET/21</t>
+          <t>K5050</t>
         </is>
       </c>
     </row>
@@ -2218,14 +2218,14 @@
         <v>28</v>
       </c>
       <c r="C105" t="n">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="D105" t="n">
-        <v>621</v>
+        <v>452</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>DEM.MEDIDA</t>
+          <t>Perdas(%)2,52,5</t>
         </is>
       </c>
     </row>
@@ -2235,14 +2235,14 @@
         <v>28</v>
       </c>
       <c r="C106" t="n">
-        <v>132</v>
+        <v>224</v>
       </c>
       <c r="D106" t="n">
-        <v>618</v>
+        <v>468</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>CONSUMOFATURADO</t>
+          <t>Fat. Pot.</t>
         </is>
       </c>
     </row>
@@ -2252,14 +2252,14 @@
         <v>28</v>
       </c>
       <c r="C107" t="n">
-        <v>163</v>
+        <v>257</v>
       </c>
       <c r="D107" t="n">
-        <v>621</v>
+        <v>468</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>DEM.MEDIDA</t>
+          <t>Aj. Fator Pot.</t>
         </is>
       </c>
     </row>
@@ -2269,14 +2269,14 @@
         <v>28</v>
       </c>
       <c r="C108" t="n">
-        <v>205</v>
+        <v>320</v>
       </c>
       <c r="D108" t="n">
-        <v>621</v>
+        <v>501</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>ERE</t>
+          <t>* K : Constante do Medidor</t>
         </is>
       </c>
     </row>
@@ -2286,14 +2286,14 @@
         <v>28</v>
       </c>
       <c r="C109" t="n">
-        <v>239</v>
+        <v>321</v>
       </c>
       <c r="D109" t="n">
-        <v>621</v>
+        <v>452</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>DRE</t>
+          <t>Dados do consumoMedido3.792,005.168,00</t>
         </is>
       </c>
     </row>
@@ -2303,14 +2303,14 @@
         <v>28</v>
       </c>
       <c r="C110" t="n">
-        <v>273</v>
+        <v>369</v>
       </c>
       <c r="D110" t="n">
-        <v>621</v>
+        <v>452</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>ERE</t>
+          <t>Faturado3.792,003.792,00</t>
         </is>
       </c>
     </row>
@@ -2320,14 +2320,14 @@
         <v>28</v>
       </c>
       <c r="C111" t="n">
-        <v>307</v>
+        <v>517</v>
       </c>
       <c r="D111" t="n">
-        <v>621</v>
+        <v>478</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>DRE</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -2337,14 +2337,14 @@
         <v>28</v>
       </c>
       <c r="C112" t="n">
-        <v>335</v>
+        <v>517</v>
       </c>
       <c r="D112" t="n">
-        <v>621</v>
+        <v>457</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>CONSUMO</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -2354,14 +2354,14 @@
         <v>28</v>
       </c>
       <c r="C113" t="n">
-        <v>375</v>
+        <v>517</v>
       </c>
       <c r="D113" t="n">
-        <v>621</v>
+        <v>438</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>ERE</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -2371,14 +2371,14 @@
         <v>28</v>
       </c>
       <c r="C114" t="n">
-        <v>113</v>
+        <v>413</v>
       </c>
       <c r="D114" t="n">
-        <v>551</v>
+        <v>432</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>4,204,204,204,204,204,204,204,204,20</t>
+          <t>DIC MENSALDIC TRIMESTRALDIC ANUALFIC MENSALFIC TRIMESTRALFIC ANUALDMICDICRI</t>
         </is>
       </c>
     </row>
@@ -2388,14 +2388,14 @@
         <v>28</v>
       </c>
       <c r="C115" t="n">
-        <v>110</v>
+        <v>468</v>
       </c>
       <c r="D115" t="n">
-        <v>528</v>
+        <v>431</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>21,00</t>
+          <t>7,000,000,003,000,000,005,0013,00</t>
         </is>
       </c>
     </row>
@@ -2405,14 +2405,14 @@
         <v>28</v>
       </c>
       <c r="C116" t="n">
-        <v>137</v>
+        <v>412</v>
       </c>
       <c r="D116" t="n">
-        <v>536</v>
+        <v>378</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>1.159,201.489,951.000,6517,85164,85205,80152,25704,551.769,251.050,002.100,00</t>
+          <t>Conjunto:CATANDUVAReferência:08/2022Tensão Contratada:Limite Adequado:</t>
         </is>
       </c>
     </row>
@@ -2422,541 +2422,14 @@
         <v>28</v>
       </c>
       <c r="C117" t="n">
-        <v>211</v>
+        <v>479</v>
       </c>
       <c r="D117" t="n">
-        <v>595</v>
+        <v>378</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>23,1014,7017,85</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="inlineStr"/>
-      <c r="B118" t="n">
-        <v>28</v>
-      </c>
-      <c r="C118" t="n">
-        <v>214</v>
-      </c>
-      <c r="D118" t="n">
-        <v>572</v>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>3,153,15</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="inlineStr"/>
-      <c r="B119" t="n">
-        <v>28</v>
-      </c>
-      <c r="C119" t="n">
-        <v>211</v>
-      </c>
-      <c r="D119" t="n">
-        <v>551</v>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>21,0070,35</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="inlineStr"/>
-      <c r="B120" t="n">
-        <v>28</v>
-      </c>
-      <c r="C120" t="n">
-        <v>180</v>
-      </c>
-      <c r="D120" t="n">
-        <v>551</v>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>8,408,408,408,408,408,404,208,408,40</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="inlineStr"/>
-      <c r="B121" t="n">
-        <v>28</v>
-      </c>
-      <c r="C121" t="n">
-        <v>178</v>
-      </c>
-      <c r="D121" t="n">
-        <v>536</v>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>10,50</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="inlineStr"/>
-      <c r="B122" t="n">
-        <v>28</v>
-      </c>
-      <c r="C122" t="n">
-        <v>276</v>
-      </c>
-      <c r="D122" t="n">
-        <v>551</v>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>197,40200,55131,254,2045,1543,0529,40142,80732,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="inlineStr"/>
-      <c r="B123" t="n">
-        <v>28</v>
-      </c>
-      <c r="C123" t="n">
-        <v>35</v>
-      </c>
-      <c r="D123" t="n">
-        <v>490</v>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>Leitura Anterior:31/08/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="inlineStr"/>
-      <c r="B124" t="n">
-        <v>28</v>
-      </c>
-      <c r="C124" t="n">
-        <v>113</v>
-      </c>
-      <c r="D124" t="n">
-        <v>490</v>
-      </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>Leitura Atual:30/09/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="inlineStr"/>
-      <c r="B125" t="n">
-        <v>28</v>
-      </c>
-      <c r="C125" t="n">
-        <v>183</v>
-      </c>
-      <c r="D125" t="n">
-        <v>490</v>
-      </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>Dias: 30</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="inlineStr"/>
-      <c r="B126" t="n">
-        <v>28</v>
-      </c>
-      <c r="C126" t="n">
-        <v>207</v>
-      </c>
-      <c r="D126" t="n">
-        <v>490</v>
-      </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>Demanda Contratada Ponta:</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="inlineStr"/>
-      <c r="B127" t="n">
-        <v>28</v>
-      </c>
-      <c r="C127" t="n">
-        <v>35</v>
-      </c>
-      <c r="D127" t="n">
-        <v>386</v>
-      </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>UN.KWHINJKWHINJKWKWEREEREDREDRE</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="inlineStr"/>
-      <c r="B128" t="n">
-        <v>28</v>
-      </c>
-      <c r="C128" t="n">
-        <v>52</v>
-      </c>
-      <c r="D128" t="n">
-        <v>468</v>
-      </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>Posto</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="inlineStr"/>
-      <c r="B129" t="n">
-        <v>28</v>
-      </c>
-      <c r="C129" t="n">
-        <v>57</v>
-      </c>
-      <c r="D129" t="n">
-        <v>386</v>
-      </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>PPFFPFPFPF</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="inlineStr"/>
-      <c r="B130" t="n">
-        <v>28</v>
-      </c>
-      <c r="C130" t="n">
-        <v>91</v>
-      </c>
-      <c r="D130" t="n">
-        <v>387</v>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>Atual0,99286,089,353.274,730,000,010,151,450,010,01</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="inlineStr"/>
-      <c r="B131" t="n">
-        <v>28</v>
-      </c>
-      <c r="C131" t="n">
-        <v>141</v>
-      </c>
-      <c r="D131" t="n">
-        <v>477</v>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>Dados da leitura</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="inlineStr"/>
-      <c r="B132" t="n">
-        <v>28</v>
-      </c>
-      <c r="C132" t="n">
-        <v>130</v>
-      </c>
-      <c r="D132" t="n">
-        <v>387</v>
-      </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>Anterior0,82275,798,243.019,500,000,000,121,270,000,00</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="inlineStr"/>
-      <c r="B133" t="n">
-        <v>28</v>
-      </c>
-      <c r="C133" t="n">
-        <v>159</v>
-      </c>
-      <c r="D133" t="n">
-        <v>387</v>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>K1050105010501050105010501050105010501050</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="inlineStr"/>
-      <c r="B134" t="n">
-        <v>28</v>
-      </c>
-      <c r="C134" t="n">
-        <v>179</v>
-      </c>
-      <c r="D134" t="n">
-        <v>387</v>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>Perdas(%)0000000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="inlineStr"/>
-      <c r="B135" t="n">
-        <v>28</v>
-      </c>
-      <c r="C135" t="n">
-        <v>224</v>
-      </c>
-      <c r="D135" t="n">
-        <v>387</v>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>Fat. Pot.0000000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="inlineStr"/>
-      <c r="B136" t="n">
-        <v>28</v>
-      </c>
-      <c r="C136" t="n">
-        <v>257</v>
-      </c>
-      <c r="D136" t="n">
-        <v>387</v>
-      </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Aj. Fator Pot.0000000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="inlineStr"/>
-      <c r="B137" t="n">
-        <v>28</v>
-      </c>
-      <c r="C137" t="n">
-        <v>318</v>
-      </c>
-      <c r="D137" t="n">
-        <v>490</v>
-      </c>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>* K : Constante do MedidorFora Ponta:</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="inlineStr"/>
-      <c r="B138" t="n">
-        <v>28</v>
-      </c>
-      <c r="C138" t="n">
-        <v>350</v>
-      </c>
-      <c r="D138" t="n">
-        <v>490</v>
-      </c>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>832,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="inlineStr"/>
-      <c r="B139" t="n">
-        <v>28</v>
-      </c>
-      <c r="C139" t="n">
-        <v>317</v>
-      </c>
-      <c r="D139" t="n">
-        <v>387</v>
-      </c>
-      <c r="E139" t="inlineStr">
-        <is>
-          <t>Dados do consumoMedido181,6510.806,601.159,20267.984,154,208,4023,10197,405,257,35</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="inlineStr"/>
-      <c r="B140" t="n">
-        <v>28</v>
-      </c>
-      <c r="C140" t="n">
-        <v>369</v>
-      </c>
-      <c r="D140" t="n">
-        <v>387</v>
-      </c>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>Faturado181,65181,651.159,201.159,200,00832,5023,10197,400,000,00</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="inlineStr"/>
-      <c r="B141" t="n">
-        <v>28</v>
-      </c>
-      <c r="C141" t="n">
-        <v>413</v>
-      </c>
-      <c r="D141" t="n">
-        <v>432</v>
-      </c>
-      <c r="E141" t="inlineStr">
-        <is>
-          <t>DIC MENSALDIC TRIMESTRALDIC ANUALFIC MENSALFIC TRIMESTRALFIC ANUALDMICDICRI</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="inlineStr"/>
-      <c r="B142" t="n">
-        <v>28</v>
-      </c>
-      <c r="C142" t="n">
-        <v>467</v>
-      </c>
-      <c r="D142" t="n">
-        <v>431</v>
-      </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>13,000,000,005,000,000,0010,0021,00</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="inlineStr"/>
-      <c r="B143" t="n">
-        <v>28</v>
-      </c>
-      <c r="C143" t="n">
-        <v>517</v>
-      </c>
-      <c r="D143" t="n">
-        <v>478</v>
-      </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>0,23</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="inlineStr"/>
-      <c r="B144" t="n">
-        <v>28</v>
-      </c>
-      <c r="C144" t="n">
-        <v>517</v>
-      </c>
-      <c r="D144" t="n">
-        <v>457</v>
-      </c>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="inlineStr"/>
-      <c r="B145" t="n">
-        <v>28</v>
-      </c>
-      <c r="C145" t="n">
-        <v>517</v>
-      </c>
-      <c r="D145" t="n">
-        <v>438</v>
-      </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>0,23</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="inlineStr"/>
-      <c r="B146" t="n">
-        <v>28</v>
-      </c>
-      <c r="C146" t="n">
-        <v>453</v>
-      </c>
-      <c r="D146" t="n">
-        <v>399</v>
-      </c>
-      <c r="E146" t="inlineStr">
-        <is>
-          <t>EXTREMA07/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="inlineStr"/>
-      <c r="B147" t="n">
-        <v>28</v>
-      </c>
-      <c r="C147" t="n">
-        <v>412</v>
-      </c>
-      <c r="D147" t="n">
-        <v>378</v>
-      </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>Conjunto:Referência:Tensão Contratada: 34500Limite Adequado:</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="inlineStr"/>
-      <c r="B148" t="n">
-        <v>28</v>
-      </c>
-      <c r="C148" t="n">
-        <v>479</v>
-      </c>
-      <c r="D148" t="n">
-        <v>378</v>
-      </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>32085 a 36225</t>
+          <t xml:space="preserve"> a</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: add openpyxl import
</commit_message>
<xml_diff>
--- a/dados_fatura.xlsx
+++ b/dados_fatura.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,7 +474,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>11:18:45</t>
+          <t>21:43:34</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PEDRO MONTELEONE VEICULOS E MOTORES LIMITADAAVENIDA ORLANDO ZANCANER, 1911 -   15801120 - 15801120INDEFINIDOCATANDUVA (AG: 401)</t>
+          <t>CONSORCIO MUNHOZ 1 ENERGIARURAL B BOM JARDIM, 0 - Sítio Paineiras, Estrada 37620000B BOM JARDIMMUNHOZ (AG: 316)</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MTC-CONVENCIONAL BAIXA TENSÃO / B3COMERCIAL / COMERCIAL</t>
+          <t>MTV-MOD.TARIFÁRIA VERDE / A3AINDUSTRIAL / INDUSTRIAL</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>003 - 4001 - 070 - 1790W9004861512</t>
+          <t>082 - 3016 - 010 - 0050W9007777164</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4025957-2022-10-5</t>
+          <t>0002598964-2022-09-4</t>
         </is>
       </c>
     </row>
@@ -589,11 +589,11 @@
         <v>211</v>
       </c>
       <c r="D9" t="n">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LIGAÇÃO:DOM.  BANC.:CNPJ/CPF/RANI: 47.069.869/0001-56Insc. Est.: 260000880111</t>
+          <t>LIGAÇÃO:DOM.  BANC.:CNPJ/CPF: 41.628.717/0001-60</t>
         </is>
       </c>
     </row>
@@ -603,14 +603,14 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>398</v>
+        <v>363</v>
       </c>
       <c r="D10" t="n">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.Rod Assis Chateaubriand S/N, KM 455 - Bairro: Vila MariaPRESIDENTE PRUDENTE – SP CEP 19053-680CNPJ 07.282.377/0001-20     Insc. Est. 562.408.684.115Nota Fiscal/Conta de Energia ElétricaSérie: U   NF: 040.936.936</t>
+          <t>ENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.Rua Capitão Soares, 667, CENTROCAMBUI - MG CEP 37600-000CNPJ 07.282.377/0081-04     Insc. Est. 002522747.04-56Nota Fiscal/Conta de Energia ElétricaSérie: B1   NF: 000.016.131Reimpressão da NF/CEE, nos termos do Regime Especial/PTA nº45.000015601-58 - SEF/MG</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Emissão: 10/10/2022</t>
+          <t>Emissão: 03/10/2022</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0004025957-4</t>
+          <t>0002598964-1</t>
         </is>
       </c>
     </row>
@@ -671,14 +671,14 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14" t="n">
         <v>674</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Outubro/2022</t>
+          <t>Setembro/2022</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14/10/2022</t>
+          <t>06/10/2022</t>
         </is>
       </c>
     </row>
@@ -705,14 +705,14 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D16" t="n">
         <v>674</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>07/11/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>9/4025957-4</t>
+          <t>9/2598964-1</t>
         </is>
       </c>
     </row>
@@ -742,11 +742,11 @@
         <v>34</v>
       </c>
       <c r="D18" t="n">
-        <v>608</v>
+        <v>568</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CCI Descrição0601 Consumo em kWh0601 Energia Atv Injetada0601 Dif. Custo Disp. Res. 482.</t>
+          <t>CCI Descrição0601 Consumo em kWh - Ponta0601 Energia Atv Injetada - Ponta0601 Consumo em kWh - Fora Ponta06010601 Energia Reativa Exced em KWh - Ponta0601 Energia Reativa Exced em KWh - FPonta0602 Demanda de Potência Medida - Fora Ponta0602 Demanda Potência Não Consumida - F Ponta</t>
         </is>
       </c>
     </row>
@@ -756,14 +756,14 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="D19" t="n">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Quantidade3.792,003.792,00100,00</t>
+          <t>Energia Atv Injetada - Fora Ponta</t>
         </is>
       </c>
     </row>
@@ -773,14 +773,14 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="D20" t="n">
-        <v>608</v>
+        <v>560</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Tarifa s/Tributos0,6219500,6219500,621950</t>
+          <t>LANÇAMENTOS E SERVIÇOS</t>
         </is>
       </c>
     </row>
@@ -790,14 +790,14 @@
         <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>257</v>
+        <v>34</v>
       </c>
       <c r="D21" t="n">
-        <v>608</v>
+        <v>552</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Tarifa c/Tributos0,7879400,7073500,787940</t>
+          <t>0807 Contrib de Ilum Pub</t>
         </is>
       </c>
     </row>
@@ -807,14 +807,14 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>293</v>
+        <v>176</v>
       </c>
       <c r="D22" t="n">
-        <v>608</v>
+        <v>568</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Valor Total(R$)2.987,88-2.682,2978,79</t>
+          <t>Quantidade181,65181,651.159,201.159,2023,10197,408,40824,10</t>
         </is>
       </c>
     </row>
@@ -824,14 +824,14 @@
         <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>332</v>
+        <v>254</v>
       </c>
       <c r="D23" t="n">
-        <v>608</v>
+        <v>568</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Base Calc.ICMS(R$)2.987,88-1.290,1378,79</t>
+          <t>Tarifa c/Tributos1,6162401,6162400,4498400,4498400,3402200,34022020,18491020,184910</t>
         </is>
       </c>
     </row>
@@ -841,14 +841,14 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>366</v>
+        <v>293</v>
       </c>
       <c r="D24" t="n">
-        <v>608</v>
+        <v>568</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>%Aliq.ICMS181818</t>
+          <t>Valor Total(R$)293,59-293,59521,47-521,477,8567,16169,5516.634,38</t>
         </is>
       </c>
     </row>
@@ -858,14 +858,14 @@
         <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>396</v>
+        <v>332</v>
       </c>
       <c r="D25" t="n">
-        <v>608</v>
+        <v>568</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ICMS (R$)537,81-232,2214,18</t>
+          <t>Base Calc.ICMS(R$)95,42-95,42374,86-374,867,8567,160,000,00</t>
         </is>
       </c>
     </row>
@@ -875,14 +875,14 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>428</v>
+        <v>366</v>
       </c>
       <c r="D26" t="n">
-        <v>641</v>
+        <v>568</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Base Calc.</t>
+          <t>%Aliq.ICMS181818181818180</t>
         </is>
       </c>
     </row>
@@ -892,14 +892,14 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>420</v>
+        <v>308</v>
       </c>
       <c r="D27" t="n">
-        <v>608</v>
+        <v>552</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>PIS/COFINS (R$)2.450,06-2.450,0664,61</t>
+          <t>46,17</t>
         </is>
       </c>
     </row>
@@ -909,14 +909,14 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>474</v>
+        <v>350</v>
       </c>
       <c r="D28" t="n">
-        <v>608</v>
+        <v>552</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>PIS (R$) COFINS(R$)(3,0729%)75,29-75,291,98</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -926,14 +926,14 @@
         <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>470</v>
+        <v>376</v>
       </c>
       <c r="D29" t="n">
-        <v>608</v>
+        <v>552</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>(0,6671%)16,34-16,340,43</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -943,14 +943,14 @@
         <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>35</v>
+        <v>400</v>
       </c>
       <c r="D30" t="n">
-        <v>431</v>
+        <v>568</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CCI: Código de Classificação do Item</t>
+          <t>ICMS (R$)17,18-17,1867,47-67,471,4112,090,000,00</t>
         </is>
       </c>
     </row>
@@ -960,14 +960,14 @@
         <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>248</v>
+        <v>405</v>
       </c>
       <c r="D31" t="n">
-        <v>431</v>
+        <v>552</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Total:</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -977,14 +977,14 @@
         <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>304</v>
+        <v>428</v>
       </c>
       <c r="D32" t="n">
-        <v>431</v>
+        <v>641</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>384,38</t>
+          <t>Base Calc.</t>
         </is>
       </c>
     </row>
@@ -994,14 +994,14 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>338</v>
+        <v>420</v>
       </c>
       <c r="D33" t="n">
-        <v>431</v>
+        <v>568</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.776,54</t>
+          <t>PIS/COFINS (R$)276,41-276,41453,99-453,996,4455,07169,5516.634,38</t>
         </is>
       </c>
     </row>
@@ -1011,14 +1011,14 @@
         <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>398</v>
+        <v>474</v>
       </c>
       <c r="D34" t="n">
-        <v>431</v>
+        <v>568</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>319,77</t>
+          <t>PIS (R$) COFINS(R$)(3,0729%)8,49-8,4913,95-13,950,201,695,21511,16</t>
         </is>
       </c>
     </row>
@@ -1028,14 +1028,14 @@
         <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>452</v>
+        <v>470</v>
       </c>
       <c r="D35" t="n">
-        <v>431</v>
+        <v>568</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>64,61</t>
+          <t>(0,6671%)1,84-1,843,03-3,030,040,371,13110,97</t>
         </is>
       </c>
     </row>
@@ -1045,14 +1045,14 @@
         <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>485</v>
+        <v>453</v>
       </c>
       <c r="D36" t="n">
-        <v>431</v>
+        <v>552</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0,43</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -1062,14 +1062,14 @@
         <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>525</v>
+        <v>485</v>
       </c>
       <c r="D37" t="n">
-        <v>431</v>
+        <v>552</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1,98</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -1079,14 +1079,14 @@
         <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>63</v>
+        <v>525</v>
       </c>
       <c r="D38" t="n">
-        <v>395</v>
+        <v>552</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>DISCRIMINAÇÃO</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>
@@ -1096,14 +1096,14 @@
         <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D39" t="n">
-        <v>355</v>
+        <v>431</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>SERVIÇO DISTRIBUIÇÃOCOMPRA DE ENERGIASERVIÇO DE TRANSMISSÃOENCARGOS SETORIAISIMPOSTOS DIRETOS E ENCARGOSOUTROS SERVIÇOS</t>
+          <t>CCI: Código de Classificação do Item</t>
         </is>
       </c>
     </row>
@@ -1113,14 +1113,14 @@
         <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>75</v>
+        <v>248</v>
       </c>
       <c r="D40" t="n">
-        <v>348</v>
+        <v>431</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>TOTAL</t>
+          <t>Total:</t>
         </is>
       </c>
     </row>
@@ -1130,14 +1130,14 @@
         <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>210</v>
+        <v>296</v>
       </c>
       <c r="D41" t="n">
-        <v>388</v>
+        <v>431</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>21/10/2022</t>
+          <t>16.925,11</t>
         </is>
       </c>
     </row>
@@ -1147,14 +1147,14 @@
         <v>4</v>
       </c>
       <c r="C42" t="n">
-        <v>382</v>
+        <v>346</v>
       </c>
       <c r="D42" t="n">
-        <v>389</v>
+        <v>431</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>R$ 384,38</t>
+          <t>75,01</t>
         </is>
       </c>
     </row>
@@ -1164,14 +1164,14 @@
         <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>137</v>
+        <v>402</v>
       </c>
       <c r="D43" t="n">
-        <v>348</v>
+        <v>431</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>VALOR (R$)12,7028,575,8815,05322,180,00384,38</t>
+          <t>13,50</t>
         </is>
       </c>
     </row>
@@ -1181,14 +1181,14 @@
         <v>4</v>
       </c>
       <c r="C44" t="n">
-        <v>172</v>
+        <v>440</v>
       </c>
       <c r="D44" t="n">
-        <v>348</v>
+        <v>431</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>%3,307,431,533,9283,820,00100,00</t>
+          <t>16.865,44</t>
         </is>
       </c>
     </row>
@@ -1198,14 +1198,14 @@
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>268</v>
+        <v>478</v>
       </c>
       <c r="D45" t="n">
-        <v>327</v>
+        <v>431</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>844d.4da2.80bd.c2de.f0fb.fa28.b32a.99a3</t>
+          <t>112,51</t>
         </is>
       </c>
     </row>
@@ -1215,14 +1215,14 @@
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>210</v>
+        <v>518</v>
       </c>
       <c r="D46" t="n">
-        <v>263</v>
+        <v>431</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>00190.00009 03268.923004 42255.211171 4 91450000038438</t>
+          <t>518,26</t>
         </is>
       </c>
     </row>
@@ -1232,14 +1232,14 @@
         <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>198</v>
+        <v>63</v>
       </c>
       <c r="D47" t="n">
-        <v>263</v>
+        <v>395</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>-9</t>
+          <t>DISCRIMINAÇÃO</t>
         </is>
       </c>
     </row>
@@ -1249,14 +1249,14 @@
         <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="D48" t="n">
-        <v>263</v>
+        <v>355</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>SERVIÇO DISTRIBUIÇÃOCOMPRA DE ENERGIASERVIÇO DE TRANSMISSÃOENCARGOS SETORIAISIMPOSTOS DIRETOS E ENCARGOSOUTROS SERVIÇOS</t>
         </is>
       </c>
     </row>
@@ -1266,14 +1266,14 @@
         <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D49" t="n">
-        <v>196</v>
+        <v>333</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>BANCO DO BRASIL S/ALOCAL DE PAGAMENTOPAGAR PREFERENCIALMENTE NO  BANCO DO BRASIL S/ABENEFICIÁRIOENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.ENDEREÇOROD ASSIS CHATEAUBRIAND S/N, S/N - KM 455 - VILA MARIA - PRESIDENTE PRUDENTE / SP - CEP 19053-680DATA DO DOCUMENTO</t>
+          <t>VALOR (R$)3.315,117.458,211.534,183.927,17690,440,0016.925,11- Valor Encargo Uso Sist. Distr. (Ref 07/2022): R$15.598,55</t>
         </is>
       </c>
     </row>
@@ -1283,14 +1283,14 @@
         <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>199</v>
+        <v>75</v>
       </c>
       <c r="D50" t="n">
-        <v>196</v>
+        <v>348</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>ESPÉCIE DOC</t>
+          <t>TOTAL</t>
         </is>
       </c>
     </row>
@@ -1300,14 +1300,14 @@
         <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>310</v>
+        <v>210</v>
       </c>
       <c r="D51" t="n">
-        <v>223</v>
+        <v>388</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>CNPJ07.282.377/0001-20</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -1317,14 +1317,14 @@
         <v>4</v>
       </c>
       <c r="C52" t="n">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="D52" t="n">
-        <v>234</v>
+        <v>389</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>VENCIMENTO21/10/2022AG./CÓD.BENEFICIÁRIO</t>
+          <t>R$ 16.925,11</t>
         </is>
       </c>
     </row>
@@ -1334,14 +1334,14 @@
         <v>4</v>
       </c>
       <c r="C53" t="n">
-        <v>453</v>
+        <v>172</v>
       </c>
       <c r="D53" t="n">
-        <v>267</v>
+        <v>348</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Promoção 1 Ano Por Nossa Conta</t>
+          <t>%19,5944,079,0623,204,080,00100,00</t>
         </is>
       </c>
     </row>
@@ -1351,14 +1351,14 @@
         <v>4</v>
       </c>
       <c r="C54" t="n">
-        <v>457</v>
+        <v>269</v>
       </c>
       <c r="D54" t="n">
-        <v>260</v>
+        <v>327</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Pague com QR Code do PIX e</t>
+          <t>8b43.8610.de33.d965.0afb.f810.cafc.ee5c</t>
         </is>
       </c>
     </row>
@@ -1368,14 +1368,14 @@
         <v>4</v>
       </c>
       <c r="C55" t="n">
-        <v>451</v>
+        <v>210</v>
       </c>
       <c r="D55" t="n">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>concorra a 1 Ano de Energia Grátis.Use seu app de pagamento favorito,</t>
+          <t>00190.00009 03268.923004 42033.164171 6 91380001692511</t>
         </is>
       </c>
     </row>
@@ -1385,14 +1385,14 @@
         <v>4</v>
       </c>
       <c r="C56" t="n">
-        <v>453</v>
+        <v>198</v>
       </c>
       <c r="D56" t="n">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>escolha "Pagar com PIX", leiao QR Code abaixo e cadastre-se:</t>
+          <t>-9</t>
         </is>
       </c>
     </row>
@@ -1402,14 +1402,14 @@
         <v>4</v>
       </c>
       <c r="C57" t="n">
-        <v>466</v>
+        <v>185</v>
       </c>
       <c r="D57" t="n">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>www.anodeconta.com.br</t>
+          <t>001</t>
         </is>
       </c>
     </row>
@@ -1419,14 +1419,14 @@
         <v>4</v>
       </c>
       <c r="C58" t="n">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D58" t="n">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>10/10/2022</t>
+          <t>BANCO DO BRASIL S/ALOCAL DE PAGAMENTOPAGAR PREFERENCIALMENTE NO  BANCO DO BRASIL S/ABENEFICIÁRIOENERGISA SUL-SUDESTE - DISTRIBUIDORA DE ENERGIA S.A.ENDEREÇOROD ASSIS CHATEAUBRIAND S/N, S/N - KM 455 - VILA MARIA - PRESIDENTE PRUDENTE / SP - CEP 19053-680DATA DO DOCUMENTO</t>
         </is>
       </c>
     </row>
@@ -1436,14 +1436,14 @@
         <v>4</v>
       </c>
       <c r="C59" t="n">
-        <v>38</v>
+        <v>199</v>
       </c>
       <c r="D59" t="n">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>USO DO BANCO</t>
+          <t>ESPÉCIE DOC</t>
         </is>
       </c>
     </row>
@@ -1453,14 +1453,14 @@
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>38</v>
+        <v>310</v>
       </c>
       <c r="D60" t="n">
-        <v>159</v>
+        <v>223</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>INSTRUÇÕES</t>
+          <t>CNPJ07.282.377/0001-20</t>
         </is>
       </c>
     </row>
@@ -1470,14 +1470,14 @@
         <v>4</v>
       </c>
       <c r="C61" t="n">
-        <v>103</v>
+        <v>373</v>
       </c>
       <c r="D61" t="n">
-        <v>169</v>
+        <v>234</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Nº DOCUMENTO4025957-2022-10-5CARTEIRA17</t>
+          <t>VENCIMENTO14/10/2022AG./CÓD.BENEFICIÁRIO</t>
         </is>
       </c>
     </row>
@@ -1487,14 +1487,14 @@
         <v>4</v>
       </c>
       <c r="C62" t="n">
-        <v>249</v>
+        <v>393</v>
       </c>
       <c r="D62" t="n">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>ACEITEN</t>
+          <t>3064-3/005292-2</t>
         </is>
       </c>
     </row>
@@ -1504,14 +1504,14 @@
         <v>4</v>
       </c>
       <c r="C63" t="n">
-        <v>286</v>
+        <v>453</v>
       </c>
       <c r="D63" t="n">
-        <v>187</v>
+        <v>267</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>DATA DO PROCESSAMENTO10/10/2022</t>
+          <t>Promoção 1 Ano Por Nossa Conta</t>
         </is>
       </c>
     </row>
@@ -1521,14 +1521,14 @@
         <v>4</v>
       </c>
       <c r="C64" t="n">
-        <v>249</v>
+        <v>457</v>
       </c>
       <c r="D64" t="n">
-        <v>177</v>
+        <v>260</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>QUANTIDADE</t>
+          <t>Pague com QR Code do PIX e</t>
         </is>
       </c>
     </row>
@@ -1538,14 +1538,14 @@
         <v>4</v>
       </c>
       <c r="C65" t="n">
-        <v>333</v>
+        <v>451</v>
       </c>
       <c r="D65" t="n">
-        <v>177</v>
+        <v>247</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>VALOR</t>
+          <t>concorra a 1 Ano de Energia Grátis.Use seu app de pagamento favorito,</t>
         </is>
       </c>
     </row>
@@ -1555,14 +1555,14 @@
         <v>4</v>
       </c>
       <c r="C66" t="n">
-        <v>215</v>
+        <v>453</v>
       </c>
       <c r="D66" t="n">
-        <v>168</v>
+        <v>233</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>DSESPÉCIER$</t>
+          <t>escolha "Pagar com PIX", leiao QR Code abaixo e cadastre-se:</t>
         </is>
       </c>
     </row>
@@ -1572,14 +1572,14 @@
         <v>4</v>
       </c>
       <c r="C67" t="n">
-        <v>38</v>
+        <v>466</v>
       </c>
       <c r="D67" t="n">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>OS VALORES DA MULTA/JUROS DE MORA POR ATRASO SÓ SERÃO COBRADOSNA PRIMEIRA FATURA APÓS O PAGAMENTO DESTA.TITULO SUJEITO A PROTESTO APÓS O VENCIMENTONÃO ACEITAMOS DEPÓSITO EM CONTA CORRENTE. CASO OCORRA, O MESMO NÃO QUITARÁ ESTA FATURA.</t>
+          <t>www.anodeconta.com.br</t>
         </is>
       </c>
     </row>
@@ -1589,14 +1589,14 @@
         <v>4</v>
       </c>
       <c r="C68" t="n">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D68" t="n">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>PAGADORPEDRO MONTELEONE VEICULOS E MOTORES LIMITADAAVENIDA ORLANDO ZANCANER, 1911 -   15801120     CATANDUVA (AG: 401)SACADOR/ AVALISTA</t>
+          <t>03/10/2022</t>
         </is>
       </c>
     </row>
@@ -1606,14 +1606,14 @@
         <v>4</v>
       </c>
       <c r="C69" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D69" t="n">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>(B{SgDgQtRuB{B{[eLcQ{B{B{LiGsSmOcB{DdMsTbWdQh)</t>
+          <t>USO DO BANCO</t>
         </is>
       </c>
     </row>
@@ -1623,14 +1623,14 @@
         <v>4</v>
       </c>
       <c r="C70" t="n">
-        <v>373</v>
+        <v>38</v>
       </c>
       <c r="D70" t="n">
-        <v>214</v>
+        <v>159</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>NOSSO NÚMERO</t>
+          <t>INSTRUÇÕES</t>
         </is>
       </c>
     </row>
@@ -1640,14 +1640,14 @@
         <v>4</v>
       </c>
       <c r="C71" t="n">
-        <v>364</v>
+        <v>103</v>
       </c>
       <c r="D71" t="n">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>32689230042255211</t>
+          <t>Nº DOCUMENTO2598964-2022-09-4CARTEIRA17</t>
         </is>
       </c>
     </row>
@@ -1657,14 +1657,14 @@
         <v>4</v>
       </c>
       <c r="C72" t="n">
-        <v>373</v>
+        <v>249</v>
       </c>
       <c r="D72" t="n">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>(=)VALOR DO DOCUMENTO</t>
+          <t>ACEITEN</t>
         </is>
       </c>
     </row>
@@ -1674,14 +1674,14 @@
         <v>4</v>
       </c>
       <c r="C73" t="n">
-        <v>373</v>
+        <v>286</v>
       </c>
       <c r="D73" t="n">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>384,38(-) DESCONTOS/ ABATIMENTOS</t>
+          <t>DATA DO PROCESSAMENTO03/10/2022</t>
         </is>
       </c>
     </row>
@@ -1691,14 +1691,14 @@
         <v>4</v>
       </c>
       <c r="C74" t="n">
-        <v>373</v>
+        <v>249</v>
       </c>
       <c r="D74" t="n">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>(-) OUTRAS DEDUÇÕES</t>
+          <t>QUANTIDADE</t>
         </is>
       </c>
     </row>
@@ -1708,14 +1708,14 @@
         <v>4</v>
       </c>
       <c r="C75" t="n">
-        <v>373</v>
+        <v>333</v>
       </c>
       <c r="D75" t="n">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>(+) MORA/ MULTA</t>
+          <t>VALOR</t>
         </is>
       </c>
     </row>
@@ -1725,14 +1725,14 @@
         <v>4</v>
       </c>
       <c r="C76" t="n">
-        <v>373</v>
+        <v>215</v>
       </c>
       <c r="D76" t="n">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>(+) OUTROS ACRÉSCIMOS</t>
+          <t>DSESPÉCIER$</t>
         </is>
       </c>
     </row>
@@ -1742,14 +1742,14 @@
         <v>4</v>
       </c>
       <c r="C77" t="n">
-        <v>373</v>
+        <v>38</v>
       </c>
       <c r="D77" t="n">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>(=) VALOR COBRADO</t>
+          <t>OS VALORES DA MULTA/JUROS DE MORA POR ATRASO SÓ SERÃO COBRADOSNA PRIMEIRA FATURA APÓS O PAGAMENTO DESTA.TITULO SUJEITO A PROTESTO APÓS O VENCIMENTONÃO ACEITAMOS DEPÓSITO EM CONTA CORRENTE. CASO OCORRA, O MESMO NÃO QUITARÁ ESTA FATURA.</t>
         </is>
       </c>
     </row>
@@ -1759,14 +1759,14 @@
         <v>4</v>
       </c>
       <c r="C78" t="n">
-        <v>373</v>
+        <v>38</v>
       </c>
       <c r="D78" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>CPF/CNPJ47.069.869/0001-56</t>
+          <t>PAGADORCONSORCIO MUNHOZ 1 ENERGIARURAL B BOM JARDIM, 0 - Sítio Paineiras, Estrada 37620000     MUNHOZ (AG: 316)SACADOR/ AVALISTA</t>
         </is>
       </c>
     </row>
@@ -1776,14 +1776,14 @@
         <v>4</v>
       </c>
       <c r="C79" t="n">
-        <v>412</v>
+        <v>39</v>
       </c>
       <c r="D79" t="n">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>CÓD. DE BAIXA</t>
+          <t>(B{SgHeYcQ{B{SsGjXbQvB{B{LiGsSmOcB{DdLi[bFrQh)</t>
         </is>
       </c>
     </row>
@@ -1793,14 +1793,14 @@
         <v>4</v>
       </c>
       <c r="C80" t="n">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D80" t="n">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>AUTENTICAÇÃO MECÂNICA</t>
+          <t>NOSSO NÚMERO</t>
         </is>
       </c>
     </row>
@@ -1810,14 +1810,14 @@
         <v>4</v>
       </c>
       <c r="C81" t="n">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D81" t="n">
-        <v>32</v>
+        <v>204</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Ficha de Compensação</t>
+          <t>32689230042033164</t>
         </is>
       </c>
     </row>
@@ -1827,14 +1827,14 @@
         <v>4</v>
       </c>
       <c r="C82" t="n">
-        <v>456</v>
+        <v>373</v>
       </c>
       <c r="D82" t="n">
-        <v>96</v>
+        <v>195</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Quer facilidade?Abra sua Conta Voltz - Energisae tenha vantagens exclusivas!</t>
+          <t>(=)VALOR DO DOCUMENTO</t>
         </is>
       </c>
     </row>
@@ -1844,184 +1844,184 @@
         <v>4</v>
       </c>
       <c r="C83" t="n">
-        <v>456</v>
+        <v>373</v>
       </c>
       <c r="D83" t="n">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Entenda melhor emcontavoltz.com/pix</t>
+          <t>16.925,11(-) DESCONTOS/ ABATIMENTOS</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr"/>
       <c r="B84" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C84" t="n">
-        <v>38</v>
+        <v>373</v>
       </c>
       <c r="D84" t="n">
-        <v>784</v>
+        <v>159</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>-Censo 2022 - Receba os recenseadores - Responda para o Brasilsaber o que precisa. censo2022.ibge.gov.br.</t>
+          <t>(-) OUTRAS DEDUÇÕES</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr"/>
       <c r="B85" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C85" t="n">
-        <v>232</v>
+        <v>373</v>
       </c>
       <c r="D85" t="n">
-        <v>790</v>
+        <v>143</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>VENCIMENTO</t>
+          <t>(+) MORA/ MULTA</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr"/>
       <c r="B86" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C86" t="n">
-        <v>277</v>
+        <v>373</v>
       </c>
       <c r="D86" t="n">
-        <v>790</v>
+        <v>126</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>VALOR (R$)</t>
+          <t>(+) OUTROS ACRÉSCIMOS</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr"/>
       <c r="B87" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C87" t="n">
-        <v>324</v>
+        <v>373</v>
       </c>
       <c r="D87" t="n">
-        <v>772</v>
+        <v>109</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Isenção Taxa IP- UC com Mini Geração conforme REH 482/2012.- Saldo Acumulado: 21099. A expirar no próximo ciclo: 0- Leitura confirmada</t>
+          <t>(=) VALOR COBRADO</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr"/>
       <c r="B88" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C88" t="n">
-        <v>52</v>
+        <v>373</v>
       </c>
       <c r="D88" t="n">
-        <v>536</v>
+        <v>84</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>MÊS/ANOOUT/22SET/22AGO/22JUL/22JUN/22MAI/22ABR/22MAR/22FEV/22JAN/22DEZ/21NOV/21OUT/21</t>
+          <t>CPF/CNPJ41.628.717/0001-60</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr"/>
       <c r="B89" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C89" t="n">
-        <v>99</v>
+        <v>412</v>
       </c>
       <c r="D89" t="n">
-        <v>635</v>
+        <v>69</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>CONVENCIONAL</t>
+          <t>CÓD. DE BAIXA</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr"/>
       <c r="B90" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C90" t="n">
-        <v>176</v>
+        <v>382</v>
       </c>
       <c r="D90" t="n">
-        <v>636</v>
+        <v>60</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>PONTA</t>
+          <t>AUTENTICAÇÃO MECÂNICA</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr"/>
       <c r="B91" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C91" t="n">
-        <v>235</v>
+        <v>373</v>
       </c>
       <c r="D91" t="n">
-        <v>635</v>
+        <v>32</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>INTERMEDIÁRIO</t>
+          <t>Ficha de Compensação</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr"/>
       <c r="B92" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C92" t="n">
-        <v>301</v>
+        <v>456</v>
       </c>
       <c r="D92" t="n">
-        <v>635</v>
+        <v>96</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>FORA  DE  PONTA</t>
+          <t>Quer facilidade?Abra sua Conta Voltz - Energisae tenha vantagens exclusivas!</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr"/>
       <c r="B93" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C93" t="n">
-        <v>184</v>
+        <v>456</v>
       </c>
       <c r="D93" t="n">
-        <v>644</v>
+        <v>76</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>HISTÓRICO DE CONSUMO (kWh)</t>
+          <t>Entenda melhor emcontavoltz.com/pix</t>
         </is>
       </c>
     </row>
@@ -2031,14 +2031,14 @@
         <v>28</v>
       </c>
       <c r="C94" t="n">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="D94" t="n">
-        <v>536</v>
+        <v>784</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>379234333741338234856303876399423613886610198881510455</t>
+          <t>-Censo 2022 - Receba os recenseadores - Responda para o Brasilsaber o que precisa. censo2022.ibge.gov.br.</t>
         </is>
       </c>
     </row>
@@ -2048,14 +2048,14 @@
         <v>28</v>
       </c>
       <c r="C95" t="n">
-        <v>35</v>
+        <v>232</v>
       </c>
       <c r="D95" t="n">
-        <v>490</v>
+        <v>790</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Leitura Anterior:06/09/2022</t>
+          <t>VENCIMENTO</t>
         </is>
       </c>
     </row>
@@ -2065,14 +2065,14 @@
         <v>28</v>
       </c>
       <c r="C96" t="n">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="D96" t="n">
-        <v>490</v>
+        <v>790</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Leitura Atual:07/10/2022</t>
+          <t>VALOR (R$)</t>
         </is>
       </c>
     </row>
@@ -2082,14 +2082,14 @@
         <v>28</v>
       </c>
       <c r="C97" t="n">
-        <v>183</v>
+        <v>324</v>
       </c>
       <c r="D97" t="n">
-        <v>490</v>
+        <v>784</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Dias: 31</t>
+          <t>UC com Mini Geração conforme REH 482/2012Saldo Ac: 5(P) 4(FP) A expirar em 10/2022: 0(P) 0(FP)</t>
         </is>
       </c>
     </row>
@@ -2099,14 +2099,14 @@
         <v>28</v>
       </c>
       <c r="C98" t="n">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D98" t="n">
-        <v>451</v>
+        <v>630</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>UN.KWHINJ</t>
+          <t>PONTA</t>
         </is>
       </c>
     </row>
@@ -2116,14 +2116,14 @@
         <v>28</v>
       </c>
       <c r="C99" t="n">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="D99" t="n">
-        <v>468</v>
+        <v>630</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Posto</t>
+          <t>FORA  DE  PONTA</t>
         </is>
       </c>
     </row>
@@ -2133,14 +2133,14 @@
         <v>28</v>
       </c>
       <c r="C100" t="n">
-        <v>57</v>
+        <v>220</v>
       </c>
       <c r="D100" t="n">
-        <v>451</v>
+        <v>630</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>PP</t>
+          <t>PONTA</t>
         </is>
       </c>
     </row>
@@ -2150,14 +2150,14 @@
         <v>28</v>
       </c>
       <c r="C101" t="n">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D101" t="n">
-        <v>452</v>
+        <v>630</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Atual927,00537,00</t>
+          <t>FORA  DE  PONTA</t>
         </is>
       </c>
     </row>
@@ -2167,14 +2167,14 @@
         <v>28</v>
       </c>
       <c r="C102" t="n">
-        <v>141</v>
+        <v>350</v>
       </c>
       <c r="D102" t="n">
-        <v>477</v>
+        <v>630</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Dados da leitura</t>
+          <t>RESERVADO</t>
         </is>
       </c>
     </row>
@@ -2184,14 +2184,14 @@
         <v>28</v>
       </c>
       <c r="C103" t="n">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="D103" t="n">
-        <v>452</v>
+        <v>551</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Anterior853,00431,00</t>
+          <t>CONSUMOFATURADO181,65128,10134,401,0512,6013,653,1598,70465,15</t>
         </is>
       </c>
     </row>
@@ -2201,14 +2201,14 @@
         <v>28</v>
       </c>
       <c r="C104" t="n">
-        <v>165</v>
+        <v>34</v>
       </c>
       <c r="D104" t="n">
-        <v>452</v>
+        <v>520</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>K5050</t>
+          <t>MÊS/ANOSET/22AGO/22JUL/22JUN/22MAI/22ABR/22MAR/22FEV/22JAN/22DEZ/21NOV/21OUT/21SET/21</t>
         </is>
       </c>
     </row>
@@ -2218,14 +2218,14 @@
         <v>28</v>
       </c>
       <c r="C105" t="n">
-        <v>179</v>
+        <v>96</v>
       </c>
       <c r="D105" t="n">
-        <v>452</v>
+        <v>621</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Perdas(%)2,52,5</t>
+          <t>DEM.MEDIDA</t>
         </is>
       </c>
     </row>
@@ -2235,14 +2235,14 @@
         <v>28</v>
       </c>
       <c r="C106" t="n">
-        <v>224</v>
+        <v>132</v>
       </c>
       <c r="D106" t="n">
-        <v>468</v>
+        <v>618</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Fat. Pot.</t>
+          <t>CONSUMOFATURADO</t>
         </is>
       </c>
     </row>
@@ -2252,14 +2252,14 @@
         <v>28</v>
       </c>
       <c r="C107" t="n">
-        <v>257</v>
+        <v>163</v>
       </c>
       <c r="D107" t="n">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Aj. Fator Pot.</t>
+          <t>DEM.MEDIDA</t>
         </is>
       </c>
     </row>
@@ -2269,14 +2269,14 @@
         <v>28</v>
       </c>
       <c r="C108" t="n">
-        <v>320</v>
+        <v>205</v>
       </c>
       <c r="D108" t="n">
-        <v>501</v>
+        <v>621</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>* K : Constante do Medidor</t>
+          <t>ERE</t>
         </is>
       </c>
     </row>
@@ -2286,14 +2286,14 @@
         <v>28</v>
       </c>
       <c r="C109" t="n">
-        <v>321</v>
+        <v>239</v>
       </c>
       <c r="D109" t="n">
-        <v>452</v>
+        <v>621</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Dados do consumoMedido3.792,005.168,00</t>
+          <t>DRE</t>
         </is>
       </c>
     </row>
@@ -2303,14 +2303,14 @@
         <v>28</v>
       </c>
       <c r="C110" t="n">
-        <v>369</v>
+        <v>273</v>
       </c>
       <c r="D110" t="n">
-        <v>452</v>
+        <v>621</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Faturado3.792,003.792,00</t>
+          <t>ERE</t>
         </is>
       </c>
     </row>
@@ -2320,14 +2320,14 @@
         <v>28</v>
       </c>
       <c r="C111" t="n">
-        <v>517</v>
+        <v>307</v>
       </c>
       <c r="D111" t="n">
-        <v>478</v>
+        <v>621</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>DRE</t>
         </is>
       </c>
     </row>
@@ -2337,14 +2337,14 @@
         <v>28</v>
       </c>
       <c r="C112" t="n">
-        <v>517</v>
+        <v>335</v>
       </c>
       <c r="D112" t="n">
-        <v>457</v>
+        <v>621</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>CONSUMO</t>
         </is>
       </c>
     </row>
@@ -2354,14 +2354,14 @@
         <v>28</v>
       </c>
       <c r="C113" t="n">
-        <v>517</v>
+        <v>375</v>
       </c>
       <c r="D113" t="n">
-        <v>438</v>
+        <v>621</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>ERE</t>
         </is>
       </c>
     </row>
@@ -2371,14 +2371,14 @@
         <v>28</v>
       </c>
       <c r="C114" t="n">
-        <v>413</v>
+        <v>113</v>
       </c>
       <c r="D114" t="n">
-        <v>432</v>
+        <v>551</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>DIC MENSALDIC TRIMESTRALDIC ANUALFIC MENSALFIC TRIMESTRALFIC ANUALDMICDICRI</t>
+          <t>4,204,204,204,204,204,204,204,204,20</t>
         </is>
       </c>
     </row>
@@ -2388,14 +2388,14 @@
         <v>28</v>
       </c>
       <c r="C115" t="n">
-        <v>468</v>
+        <v>110</v>
       </c>
       <c r="D115" t="n">
-        <v>431</v>
+        <v>528</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>7,000,000,003,000,000,005,0013,00</t>
+          <t>21,00</t>
         </is>
       </c>
     </row>
@@ -2405,14 +2405,14 @@
         <v>28</v>
       </c>
       <c r="C116" t="n">
-        <v>412</v>
+        <v>137</v>
       </c>
       <c r="D116" t="n">
-        <v>378</v>
+        <v>536</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Conjunto:CATANDUVAReferência:08/2022Tensão Contratada:Limite Adequado:</t>
+          <t>1.159,201.489,951.000,6517,85164,85205,80152,25704,551.769,251.050,002.100,00</t>
         </is>
       </c>
     </row>
@@ -2422,14 +2422,541 @@
         <v>28</v>
       </c>
       <c r="C117" t="n">
+        <v>211</v>
+      </c>
+      <c r="D117" t="n">
+        <v>595</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>23,1014,7017,85</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr"/>
+      <c r="B118" t="n">
+        <v>28</v>
+      </c>
+      <c r="C118" t="n">
+        <v>214</v>
+      </c>
+      <c r="D118" t="n">
+        <v>572</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>3,153,15</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr"/>
+      <c r="B119" t="n">
+        <v>28</v>
+      </c>
+      <c r="C119" t="n">
+        <v>211</v>
+      </c>
+      <c r="D119" t="n">
+        <v>551</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>21,0070,35</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr"/>
+      <c r="B120" t="n">
+        <v>28</v>
+      </c>
+      <c r="C120" t="n">
+        <v>180</v>
+      </c>
+      <c r="D120" t="n">
+        <v>551</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>8,408,408,408,408,408,404,208,408,40</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr"/>
+      <c r="B121" t="n">
+        <v>28</v>
+      </c>
+      <c r="C121" t="n">
+        <v>178</v>
+      </c>
+      <c r="D121" t="n">
+        <v>536</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>10,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr"/>
+      <c r="B122" t="n">
+        <v>28</v>
+      </c>
+      <c r="C122" t="n">
+        <v>276</v>
+      </c>
+      <c r="D122" t="n">
+        <v>551</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>197,40200,55131,254,2045,1543,0529,40142,80732,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr"/>
+      <c r="B123" t="n">
+        <v>28</v>
+      </c>
+      <c r="C123" t="n">
+        <v>35</v>
+      </c>
+      <c r="D123" t="n">
+        <v>490</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Leitura Anterior:31/08/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr"/>
+      <c r="B124" t="n">
+        <v>28</v>
+      </c>
+      <c r="C124" t="n">
+        <v>113</v>
+      </c>
+      <c r="D124" t="n">
+        <v>490</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Leitura Atual:30/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr"/>
+      <c r="B125" t="n">
+        <v>28</v>
+      </c>
+      <c r="C125" t="n">
+        <v>183</v>
+      </c>
+      <c r="D125" t="n">
+        <v>490</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Dias: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr"/>
+      <c r="B126" t="n">
+        <v>28</v>
+      </c>
+      <c r="C126" t="n">
+        <v>207</v>
+      </c>
+      <c r="D126" t="n">
+        <v>490</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Demanda Contratada Ponta:</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr"/>
+      <c r="B127" t="n">
+        <v>28</v>
+      </c>
+      <c r="C127" t="n">
+        <v>35</v>
+      </c>
+      <c r="D127" t="n">
+        <v>386</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>UN.KWHINJKWHINJKWKWEREEREDREDRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr"/>
+      <c r="B128" t="n">
+        <v>28</v>
+      </c>
+      <c r="C128" t="n">
+        <v>52</v>
+      </c>
+      <c r="D128" t="n">
+        <v>468</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Posto</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr"/>
+      <c r="B129" t="n">
+        <v>28</v>
+      </c>
+      <c r="C129" t="n">
+        <v>57</v>
+      </c>
+      <c r="D129" t="n">
+        <v>386</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>PPFFPFPFPF</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr"/>
+      <c r="B130" t="n">
+        <v>28</v>
+      </c>
+      <c r="C130" t="n">
+        <v>91</v>
+      </c>
+      <c r="D130" t="n">
+        <v>387</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Atual0,99286,089,353.274,730,000,010,151,450,010,01</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr"/>
+      <c r="B131" t="n">
+        <v>28</v>
+      </c>
+      <c r="C131" t="n">
+        <v>141</v>
+      </c>
+      <c r="D131" t="n">
+        <v>477</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Dados da leitura</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr"/>
+      <c r="B132" t="n">
+        <v>28</v>
+      </c>
+      <c r="C132" t="n">
+        <v>130</v>
+      </c>
+      <c r="D132" t="n">
+        <v>387</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Anterior0,82275,798,243.019,500,000,000,121,270,000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr"/>
+      <c r="B133" t="n">
+        <v>28</v>
+      </c>
+      <c r="C133" t="n">
+        <v>159</v>
+      </c>
+      <c r="D133" t="n">
+        <v>387</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>K1050105010501050105010501050105010501050</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr"/>
+      <c r="B134" t="n">
+        <v>28</v>
+      </c>
+      <c r="C134" t="n">
+        <v>179</v>
+      </c>
+      <c r="D134" t="n">
+        <v>387</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Perdas(%)0000000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="inlineStr"/>
+      <c r="B135" t="n">
+        <v>28</v>
+      </c>
+      <c r="C135" t="n">
+        <v>224</v>
+      </c>
+      <c r="D135" t="n">
+        <v>387</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Fat. Pot.0000000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr"/>
+      <c r="B136" t="n">
+        <v>28</v>
+      </c>
+      <c r="C136" t="n">
+        <v>257</v>
+      </c>
+      <c r="D136" t="n">
+        <v>387</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Aj. Fator Pot.0000000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="inlineStr"/>
+      <c r="B137" t="n">
+        <v>28</v>
+      </c>
+      <c r="C137" t="n">
+        <v>318</v>
+      </c>
+      <c r="D137" t="n">
+        <v>490</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>* K : Constante do MedidorFora Ponta:</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="inlineStr"/>
+      <c r="B138" t="n">
+        <v>28</v>
+      </c>
+      <c r="C138" t="n">
+        <v>350</v>
+      </c>
+      <c r="D138" t="n">
+        <v>490</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>832,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="inlineStr"/>
+      <c r="B139" t="n">
+        <v>28</v>
+      </c>
+      <c r="C139" t="n">
+        <v>317</v>
+      </c>
+      <c r="D139" t="n">
+        <v>387</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Dados do consumoMedido181,6510.806,601.159,20267.984,154,208,4023,10197,405,257,35</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="inlineStr"/>
+      <c r="B140" t="n">
+        <v>28</v>
+      </c>
+      <c r="C140" t="n">
+        <v>369</v>
+      </c>
+      <c r="D140" t="n">
+        <v>387</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Faturado181,65181,651.159,201.159,200,00832,5023,10197,400,000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr"/>
+      <c r="B141" t="n">
+        <v>28</v>
+      </c>
+      <c r="C141" t="n">
+        <v>413</v>
+      </c>
+      <c r="D141" t="n">
+        <v>432</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>DIC MENSALDIC TRIMESTRALDIC ANUALFIC MENSALFIC TRIMESTRALFIC ANUALDMICDICRI</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="inlineStr"/>
+      <c r="B142" t="n">
+        <v>28</v>
+      </c>
+      <c r="C142" t="n">
+        <v>467</v>
+      </c>
+      <c r="D142" t="n">
+        <v>431</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>13,000,000,005,000,000,0010,0021,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="inlineStr"/>
+      <c r="B143" t="n">
+        <v>28</v>
+      </c>
+      <c r="C143" t="n">
+        <v>517</v>
+      </c>
+      <c r="D143" t="n">
+        <v>478</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>0,23</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="inlineStr"/>
+      <c r="B144" t="n">
+        <v>28</v>
+      </c>
+      <c r="C144" t="n">
+        <v>517</v>
+      </c>
+      <c r="D144" t="n">
+        <v>457</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr"/>
+      <c r="B145" t="n">
+        <v>28</v>
+      </c>
+      <c r="C145" t="n">
+        <v>517</v>
+      </c>
+      <c r="D145" t="n">
+        <v>438</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>0,23</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr"/>
+      <c r="B146" t="n">
+        <v>28</v>
+      </c>
+      <c r="C146" t="n">
+        <v>453</v>
+      </c>
+      <c r="D146" t="n">
+        <v>399</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>EXTREMA07/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr"/>
+      <c r="B147" t="n">
+        <v>28</v>
+      </c>
+      <c r="C147" t="n">
+        <v>412</v>
+      </c>
+      <c r="D147" t="n">
+        <v>378</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Conjunto:Referência:Tensão Contratada: 34500Limite Adequado:</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr"/>
+      <c r="B148" t="n">
+        <v>28</v>
+      </c>
+      <c r="C148" t="n">
         <v>479</v>
       </c>
-      <c r="D117" t="n">
+      <c r="D148" t="n">
         <v>378</v>
       </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> a</t>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>32085 a 36225</t>
         </is>
       </c>
     </row>

</xml_diff>